<commit_message>
gradle update and backup option
</commit_message>
<xml_diff>
--- a/assets/clientList.xlsx
+++ b/assets/clientList.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">RegistrationId</t>
   </si>
@@ -31,6 +31,9 @@
     <t xml:space="preserve">FathersName</t>
   </si>
   <si>
+    <t xml:space="preserve">Dob(DDMMYYYY)</t>
+  </si>
+  <si>
     <t xml:space="preserve">MobileNo</t>
   </si>
   <si>
@@ -58,7 +61,10 @@
     <t xml:space="preserve">Weight</t>
   </si>
   <si>
-    <t xml:space="preserve">Due</t>
+    <t xml:space="preserve">NoOfPayments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StartDate(DDMMYYYY)</t>
   </si>
 </sst>
 </file>
@@ -68,7 +74,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -103,6 +109,12 @@
       <name val="DejaVu Sans Mono"/>
       <family val="3"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -147,7 +159,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -157,6 +169,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -177,17 +193,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="5.38"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1020" min="3" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.79"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="5" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="15.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="21.36"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="16" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -200,7 +221,7 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -229,6 +250,12 @@
       </c>
       <c r="M1" s="2" t="s">
         <v>12</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>